<commit_message>
not nesessyry files were deleted
</commit_message>
<xml_diff>
--- a/preise.xlsx
+++ b/preise.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://paisiihilendarskimunchen.sharepoint.com/sites/management/Shared Documents/General/20 Администрация/10 Финанси/40 Quittung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Workspace\bg-school-certificate-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{FD098EB4-1189-4E12-A66A-B254A9BAD95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61EAD950-CECB-4F9C-970B-3B2B4BFF3C3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA535B3-DE50-42FB-B983-A802547D30DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Beitraege" sheetId="1" r:id="rId1"/>
-    <sheet name="Konfiguration" sheetId="3" r:id="rId2"/>
+    <sheet name="Konfiguration" sheetId="3" r:id="rId1"/>
+    <sheet name="Beitraege" sheetId="1" r:id="rId2"/>
     <sheet name="Gebuehren" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Kind_Nr</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>2024/2025</t>
+  </si>
+  <si>
+    <t>Rechnungsstartindex</t>
   </si>
 </sst>
 </file>
@@ -394,6 +397,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE60E8-AF1D-4A2A-987F-130640E02E75}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -442,37 +487,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE60E8-AF1D-4A2A-987F-130640E02E75}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74978CF-B58C-4F9A-B63A-B7C10EF99CCA}">
   <dimension ref="A1:B4"/>
@@ -522,14 +536,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69b70055-4ccd-41e5-ba44-04aa7b40ef87">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d7d4427-3d9a-4210-88a6-80411ae356c7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,21 +740,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69b70055-4ccd-41e5-ba44-04aa7b40ef87">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d7d4427-3d9a-4210-88a6-80411ae356c7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E074D9-8A3F-4B12-8FF2-84C884A0412A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A75E2A0C-A03D-4EF1-AA2F-BC86D3F36961}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="69b70055-4ccd-41e5-ba44-04aa7b40ef87"/>
-    <ds:schemaRef ds:uri="0d7d4427-3d9a-4210-88a6-80411ae356c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -767,9 +778,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A75E2A0C-A03D-4EF1-AA2F-BC86D3F36961}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E074D9-8A3F-4B12-8FF2-84C884A0412A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="69b70055-4ccd-41e5-ba44-04aa7b40ef87"/>
+    <ds:schemaRef ds:uri="0d7d4427-3d9a-4210-88a6-80411ae356c7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>